<commit_message>
plein de modifs sur calcul avg
</commit_message>
<xml_diff>
--- a/Documentation/features director.xlsx
+++ b/Documentation/features director.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapno\Documents\moviesIA\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
   <si>
     <t>Field_name</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War','Family','Music','History','TV Movie','Foreign',</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -422,11 +425,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H61"/>
+  <dimension ref="B2:H63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,7 +941,7 @@
       <c r="G9" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -960,7 +964,7 @@
       <c r="G10" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -977,13 +981,13 @@
       <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="9">
         <v>20</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1000,11 +1004,11 @@
       <c r="E12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1021,11 +1025,11 @@
       <c r="E13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1065,7 +1069,7 @@
         <f>C28</f>
         <v>216831</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <f>D18/$C$16</f>
         <v>0.65906079027355624</v>
       </c>
@@ -1081,7 +1085,7 @@
         <f>C29</f>
         <v>20465</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f t="shared" ref="E19:E26" si="0">D19/$C$16</f>
         <v>6.2203647416413377E-2</v>
       </c>
@@ -1097,7 +1101,7 @@
         <f>C30</f>
         <v>14734</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <f t="shared" si="0"/>
         <v>4.478419452887538E-2</v>
       </c>
@@ -1113,7 +1117,7 @@
         <f>C31+C34</f>
         <v>18851</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <f t="shared" si="0"/>
         <v>5.7297872340425535E-2</v>
       </c>
@@ -1129,7 +1133,7 @@
         <f>C32</f>
         <v>8393</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <f t="shared" si="0"/>
         <v>2.551063829787234E-2</v>
       </c>
@@ -1145,7 +1149,7 @@
         <f>C33</f>
         <v>7749</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <f t="shared" si="0"/>
         <v>2.3553191489361702E-2</v>
       </c>
@@ -1161,7 +1165,7 @@
         <f>C38</f>
         <v>2891</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <f t="shared" si="0"/>
         <v>8.7872340425531915E-3</v>
       </c>
@@ -1177,7 +1181,7 @@
         <f>C40+C39</f>
         <v>4260</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <f t="shared" si="0"/>
         <v>1.2948328267477204E-2</v>
       </c>
@@ -1193,7 +1197,7 @@
         <f>C16-SUM(D18:D25)</f>
         <v>34826</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <f t="shared" si="0"/>
         <v>0.10585410334346504</v>
       </c>
@@ -1311,100 +1315,185 @@
       <c r="B42" s="6" t="s">
         <v>69</v>
       </c>
+      <c r="C42" t="str">
+        <f>CONCATENATE("'",B42,"',")</f>
+        <v>'Drama',</v>
+      </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="6" t="s">
         <v>70</v>
       </c>
+      <c r="C43" t="str">
+        <f>CONCATENATE(C42,"'",B43,"',")</f>
+        <v>'Drama','Crime',</v>
+      </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="C44" t="str">
+        <f t="shared" ref="C44:C61" si="1">CONCATENATE(C43,"'",B44,"',")</f>
+        <v>'Drama','Crime','Action',</v>
+      </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="C45" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary',</v>
+      </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
         <v>73</v>
       </c>
+      <c r="C46" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure',</v>
+      </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="C47" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation',</v>
+      </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy',</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery',</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C50" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror',</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C51" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western',</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C52" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction',</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C53" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller',</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C54" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance',</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C55" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy',</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C56" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War',</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C57" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War','Family',</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C58" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War','Family','Music',</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C59" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War','Family','Music','History',</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C60" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War','Family','Music','History','TV Movie',</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="6" t="s">
         <v>88</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="1"/>
+        <v>'Drama','Crime','Action','Documentary','Adventure','Animation','Comedy','Mystery','Horror','Western','Science Fiction','Thriller','Romance','Fantasy','War','Family','Music','History','TV Movie','Foreign',</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C63" s="10" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>